<commit_message>
Update Journal de travail Bataille Navale Rui_Monteiro.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
+++ b/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rui-Miguel.MONTEIRO\Google Drive\CPNV\1ére année\Modules\ICT\431\Bataille Navale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1.Modules\MA\20\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t xml:space="preserve">Mise en ligne la documentation </t>
+  </si>
+  <si>
+    <t>J'ai crée les dossiers de documentations (use case, journal de travail)</t>
+  </si>
+  <si>
+    <t>J'ai commencé les modifications dans ma documentation ansi a réflechir comment coder la BatailleNavale</t>
   </si>
 </sst>
 </file>
@@ -361,6 +367,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -378,21 +399,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -677,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -688,7 +694,7 @@
     <col min="3" max="5" width="11.5703125" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="2" customWidth="1"/>
     <col min="7" max="10" width="17.140625" style="2"/>
-    <col min="11" max="11" width="53.42578125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="53.42578125" style="11" customWidth="1"/>
     <col min="12" max="12" width="1.42578125" style="7" customWidth="1"/>
     <col min="13" max="16384" width="17.140625" style="2"/>
   </cols>
@@ -703,33 +709,33 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
-      <c r="K1" s="15"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="11"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16"/>
     </row>
     <row r="3" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="14"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="19"/>
     </row>
     <row r="4" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
@@ -759,7 +765,7 @@
       <c r="J4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -790,10 +796,12 @@
       <c r="I5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="18"/>
-    </row>
-    <row r="6" spans="2:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="2:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <f ca="1">TODAY()</f>
         <v>44244</v>
@@ -820,8 +828,10 @@
       <c r="I6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="18" t="s">
+      <c r="J6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="12" t="s">
         <v>25</v>
       </c>
     </row>
@@ -853,7 +863,7 @@
         <v>23</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="18"/>
+      <c r="K7" s="12"/>
     </row>
     <row r="8" spans="2:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
@@ -883,7 +893,7 @@
         <v>23</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="18"/>
+      <c r="K8" s="12"/>
     </row>
     <row r="9" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
@@ -913,7 +923,7 @@
         <v>23</v>
       </c>
       <c r="J9" s="5"/>
-      <c r="K9" s="18"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" spans="2:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
@@ -943,7 +953,7 @@
         <v>23</v>
       </c>
       <c r="J10" s="5"/>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="12" t="s">
         <v>32</v>
       </c>
     </row>
@@ -975,7 +985,7 @@
         <v>23</v>
       </c>
       <c r="J11" s="5"/>
-      <c r="K11" s="18"/>
+      <c r="K11" s="12"/>
     </row>
     <row r="12" spans="2:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
@@ -1005,268 +1015,268 @@
         <v>23</v>
       </c>
       <c r="J12" s="5"/>
-      <c r="K12" s="18"/>
+      <c r="K12" s="12"/>
     </row>
     <row r="13" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K13" s="19"/>
+      <c r="K13" s="13"/>
     </row>
     <row r="14" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K14" s="19"/>
+      <c r="K14" s="13"/>
     </row>
     <row r="15" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K15" s="19"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K16" s="19"/>
+      <c r="K16" s="13"/>
     </row>
     <row r="17" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K17" s="19"/>
+      <c r="K17" s="13"/>
     </row>
     <row r="18" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K18" s="19"/>
+      <c r="K18" s="13"/>
     </row>
     <row r="19" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K19" s="19"/>
+      <c r="K19" s="13"/>
     </row>
     <row r="20" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K20" s="19"/>
+      <c r="K20" s="13"/>
     </row>
     <row r="21" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K21" s="19"/>
+      <c r="K21" s="13"/>
     </row>
     <row r="22" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K22" s="19"/>
+      <c r="K22" s="13"/>
     </row>
     <row r="23" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K23" s="19"/>
+      <c r="K23" s="13"/>
     </row>
     <row r="24" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K24" s="19"/>
+      <c r="K24" s="13"/>
     </row>
     <row r="25" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K25" s="19"/>
+      <c r="K25" s="13"/>
     </row>
     <row r="26" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K26" s="19"/>
+      <c r="K26" s="13"/>
     </row>
     <row r="27" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K27" s="19"/>
+      <c r="K27" s="13"/>
     </row>
     <row r="28" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K28" s="19"/>
+      <c r="K28" s="13"/>
     </row>
     <row r="29" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K29" s="19"/>
+      <c r="K29" s="13"/>
     </row>
     <row r="30" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K30" s="19"/>
+      <c r="K30" s="13"/>
     </row>
     <row r="31" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K31" s="19"/>
+      <c r="K31" s="13"/>
     </row>
     <row r="32" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K32" s="19"/>
+      <c r="K32" s="13"/>
     </row>
     <row r="33" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K33" s="19"/>
+      <c r="K33" s="13"/>
     </row>
     <row r="34" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K34" s="19"/>
+      <c r="K34" s="13"/>
     </row>
     <row r="35" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K35" s="19"/>
+      <c r="K35" s="13"/>
     </row>
     <row r="36" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K36" s="19"/>
+      <c r="K36" s="13"/>
     </row>
     <row r="37" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K37" s="19"/>
+      <c r="K37" s="13"/>
     </row>
     <row r="38" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K38" s="19"/>
+      <c r="K38" s="13"/>
     </row>
     <row r="39" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K39" s="19"/>
+      <c r="K39" s="13"/>
     </row>
     <row r="40" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K40" s="19"/>
+      <c r="K40" s="13"/>
     </row>
     <row r="41" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K41" s="19"/>
+      <c r="K41" s="13"/>
     </row>
     <row r="42" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K42" s="19"/>
+      <c r="K42" s="13"/>
     </row>
     <row r="43" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K43" s="19"/>
+      <c r="K43" s="13"/>
     </row>
     <row r="44" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K44" s="19"/>
+      <c r="K44" s="13"/>
     </row>
     <row r="45" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K45" s="19"/>
+      <c r="K45" s="13"/>
     </row>
     <row r="46" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K46" s="19"/>
+      <c r="K46" s="13"/>
     </row>
     <row r="47" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K47" s="19"/>
+      <c r="K47" s="13"/>
     </row>
     <row r="48" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K48" s="19"/>
+      <c r="K48" s="13"/>
     </row>
     <row r="49" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K49" s="19"/>
+      <c r="K49" s="13"/>
     </row>
     <row r="50" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K50" s="19"/>
+      <c r="K50" s="13"/>
     </row>
     <row r="51" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K51" s="19"/>
+      <c r="K51" s="13"/>
     </row>
     <row r="52" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K52" s="19"/>
+      <c r="K52" s="13"/>
     </row>
     <row r="53" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K53" s="19"/>
+      <c r="K53" s="13"/>
     </row>
     <row r="54" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K54" s="19"/>
+      <c r="K54" s="13"/>
     </row>
     <row r="55" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K55" s="19"/>
+      <c r="K55" s="13"/>
     </row>
     <row r="56" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K56" s="19"/>
+      <c r="K56" s="13"/>
     </row>
     <row r="57" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K57" s="19"/>
+      <c r="K57" s="13"/>
     </row>
     <row r="58" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K58" s="19"/>
+      <c r="K58" s="13"/>
     </row>
     <row r="59" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K59" s="19"/>
+      <c r="K59" s="13"/>
     </row>
     <row r="60" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K60" s="19"/>
+      <c r="K60" s="13"/>
     </row>
     <row r="61" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K61" s="19"/>
+      <c r="K61" s="13"/>
     </row>
     <row r="62" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K62" s="19"/>
+      <c r="K62" s="13"/>
     </row>
     <row r="63" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K63" s="19"/>
+      <c r="K63" s="13"/>
     </row>
     <row r="64" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K64" s="19"/>
+      <c r="K64" s="13"/>
     </row>
     <row r="65" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K65" s="19"/>
+      <c r="K65" s="13"/>
     </row>
     <row r="66" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K66" s="19"/>
+      <c r="K66" s="13"/>
     </row>
     <row r="67" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K67" s="19"/>
+      <c r="K67" s="13"/>
     </row>
     <row r="68" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K68" s="19"/>
+      <c r="K68" s="13"/>
     </row>
     <row r="69" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K69" s="19"/>
+      <c r="K69" s="13"/>
     </row>
     <row r="70" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K70" s="19"/>
+      <c r="K70" s="13"/>
     </row>
     <row r="71" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K71" s="19"/>
+      <c r="K71" s="13"/>
     </row>
     <row r="72" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K72" s="19"/>
+      <c r="K72" s="13"/>
     </row>
     <row r="73" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K73" s="19"/>
+      <c r="K73" s="13"/>
     </row>
     <row r="74" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K74" s="19"/>
+      <c r="K74" s="13"/>
     </row>
     <row r="75" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K75" s="19"/>
+      <c r="K75" s="13"/>
     </row>
     <row r="76" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K76" s="19"/>
+      <c r="K76" s="13"/>
     </row>
     <row r="77" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K77" s="19"/>
+      <c r="K77" s="13"/>
     </row>
     <row r="78" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K78" s="19"/>
+      <c r="K78" s="13"/>
     </row>
     <row r="79" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K79" s="19"/>
+      <c r="K79" s="13"/>
     </row>
     <row r="80" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K80" s="19"/>
+      <c r="K80" s="13"/>
     </row>
     <row r="81" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K81" s="19"/>
+      <c r="K81" s="13"/>
     </row>
     <row r="82" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K82" s="19"/>
+      <c r="K82" s="13"/>
     </row>
     <row r="83" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K83" s="19"/>
+      <c r="K83" s="13"/>
     </row>
     <row r="84" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K84" s="19"/>
+      <c r="K84" s="13"/>
     </row>
     <row r="85" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K85" s="19"/>
+      <c r="K85" s="13"/>
     </row>
     <row r="86" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K86" s="19"/>
+      <c r="K86" s="13"/>
     </row>
     <row r="87" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K87" s="19"/>
+      <c r="K87" s="13"/>
     </row>
     <row r="88" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K88" s="19"/>
+      <c r="K88" s="13"/>
     </row>
     <row r="89" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K89" s="19"/>
+      <c r="K89" s="13"/>
     </row>
     <row r="90" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K90" s="19"/>
+      <c r="K90" s="13"/>
     </row>
     <row r="91" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K91" s="19"/>
+      <c r="K91" s="13"/>
     </row>
     <row r="92" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K92" s="19"/>
+      <c r="K92" s="13"/>
     </row>
     <row r="93" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K93" s="19"/>
+      <c r="K93" s="13"/>
     </row>
     <row r="94" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K94" s="19"/>
+      <c r="K94" s="13"/>
     </row>
     <row r="95" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K95" s="19"/>
+      <c r="K95" s="13"/>
     </row>
     <row r="96" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K96" s="19"/>
+      <c r="K96" s="13"/>
     </row>
     <row r="97" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K97" s="19"/>
+      <c r="K97" s="13"/>
     </row>
     <row r="98" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K98" s="19"/>
+      <c r="K98" s="13"/>
     </row>
     <row r="99" spans="11:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K99" s="19"/>
+      <c r="K99" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Amélioration de la documentation puis README
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
+++ b/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -164,6 +164,18 @@
   </si>
   <si>
     <t>Commencé le MCD pourtant je crois qu'il me manque encore des tables que je matterais a jour.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explication du cdc (cahier des charges) </t>
+  </si>
+  <si>
+    <t>Avec M.Viret on a revu les dates dans les quelles on deverá livrer chaq'une des parties du code ainsi que les documents</t>
+  </si>
+  <si>
+    <t>Amélioration de la documentation et commencé une base d'un README</t>
+  </si>
+  <si>
+    <t>J'ai continué de penser a quoi faire dans ma documentation, quoi écrire, puis j'ai compplété mon README dans GitHub</t>
   </si>
 </sst>
 </file>
@@ -172,7 +184,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -401,6 +413,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -417,9 +432,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -705,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -734,30 +746,30 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="17"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
     </row>
     <row r="4" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
@@ -792,7 +804,7 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="18">
+      <c r="B5" s="12">
         <v>44238</v>
       </c>
       <c r="C5" s="5">
@@ -823,7 +835,7 @@
       <c r="K5" s="11"/>
     </row>
     <row r="6" spans="2:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="18">
+      <c r="B6" s="12">
         <v>44238</v>
       </c>
       <c r="C6" s="5">
@@ -856,7 +868,7 @@
       </c>
     </row>
     <row r="7" spans="2:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18">
+      <c r="B7" s="12">
         <v>44238</v>
       </c>
       <c r="C7" s="5">
@@ -885,7 +897,7 @@
       <c r="K7" s="11"/>
     </row>
     <row r="8" spans="2:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18">
+      <c r="B8" s="12">
         <v>44238</v>
       </c>
       <c r="C8" s="5">
@@ -914,7 +926,7 @@
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18">
+      <c r="B9" s="12">
         <v>44244</v>
       </c>
       <c r="C9" s="5">
@@ -943,7 +955,7 @@
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="2:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18">
+      <c r="B10" s="12">
         <v>44244</v>
       </c>
       <c r="C10" s="5">
@@ -974,7 +986,7 @@
       </c>
     </row>
     <row r="11" spans="2:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="18">
+      <c r="B11" s="12">
         <v>44244</v>
       </c>
       <c r="C11" s="5">
@@ -1003,7 +1015,7 @@
       <c r="K11" s="11"/>
     </row>
     <row r="12" spans="2:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="18">
+      <c r="B12" s="12">
         <v>44244</v>
       </c>
       <c r="C12" s="5">
@@ -1032,7 +1044,7 @@
       <c r="K12" s="11"/>
     </row>
     <row r="13" spans="2:11" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18">
+      <c r="B13" s="12">
         <v>44245</v>
       </c>
       <c r="C13" s="5">
@@ -1063,7 +1075,7 @@
       <c r="K13" s="11"/>
     </row>
     <row r="14" spans="2:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="18">
+      <c r="B14" s="12">
         <v>44245</v>
       </c>
       <c r="C14" s="5">
@@ -1094,7 +1106,7 @@
       <c r="K14" s="11"/>
     </row>
     <row r="15" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="18">
+      <c r="B15" s="12">
         <v>44245</v>
       </c>
       <c r="C15" s="5">
@@ -1127,7 +1139,7 @@
       </c>
     </row>
     <row r="16" spans="2:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="18">
+      <c r="B16" s="12">
         <v>44245</v>
       </c>
       <c r="C16" s="5">
@@ -1137,7 +1149,7 @@
         <v>42217.510416666664</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" ref="E14:E77" si="6">D16-C16</f>
+        <f t="shared" ref="E16:E77" si="6">D16-C16</f>
         <v>5.2083333328482695E-2</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -1157,54 +1169,68 @@
       </c>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
+    <row r="17" spans="2:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="12">
+        <v>44246</v>
+      </c>
       <c r="C17" s="5">
-        <v>42217</v>
+        <v>42217.5625</v>
       </c>
       <c r="D17" s="5">
-        <v>42217</v>
+        <v>42217.583333333336</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="4"/>
+        <v>2.0833333335758653E-2</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="I17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="4"/>
+      <c r="J17" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18"/>
+    <row r="18" spans="2:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
       <c r="C18" s="5">
-        <v>42217</v>
+        <v>42217.583333333336</v>
       </c>
       <c r="D18" s="5">
-        <v>42217</v>
+        <v>42217.628472222219</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="4"/>
+        <v>4.5138888883229811E-2</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="G18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="I18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="K18" s="11"/>
     </row>
     <row r="19" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="5">
         <v>42217</v>
       </c>
@@ -1227,7 +1253,7 @@
       <c r="K19" s="11"/>
     </row>
     <row r="20" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="5">
         <v>42217</v>
       </c>
@@ -1250,7 +1276,7 @@
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="18"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="5">
         <v>42217</v>
       </c>
@@ -1273,7 +1299,7 @@
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="5">
         <v>42217</v>
       </c>
@@ -1296,7 +1322,7 @@
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="18"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="5">
         <v>42217</v>
       </c>
@@ -1319,7 +1345,7 @@
       <c r="K23" s="11"/>
     </row>
     <row r="24" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="18"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="5">
         <v>42217</v>
       </c>
@@ -1342,7 +1368,7 @@
       <c r="K24" s="11"/>
     </row>
     <row r="25" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="18"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="5">
         <v>42217</v>
       </c>
@@ -1365,7 +1391,7 @@
       <c r="K25" s="11"/>
     </row>
     <row r="26" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="18"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="5">
         <v>42217</v>
       </c>
@@ -1388,7 +1414,7 @@
       <c r="K26" s="11"/>
     </row>
     <row r="27" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="18"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="5">
         <v>42217</v>
       </c>
@@ -1411,7 +1437,7 @@
       <c r="K27" s="11"/>
     </row>
     <row r="28" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="18"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="5">
         <v>42217</v>
       </c>
@@ -1434,7 +1460,7 @@
       <c r="K28" s="11"/>
     </row>
     <row r="29" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="18"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="5">
         <v>42217</v>
       </c>
@@ -1457,7 +1483,7 @@
       <c r="K29" s="11"/>
     </row>
     <row r="30" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="18"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="5">
         <v>42217</v>
       </c>
@@ -1480,7 +1506,7 @@
       <c r="K30" s="11"/>
     </row>
     <row r="31" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="18"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="5">
         <v>42217</v>
       </c>
@@ -1503,7 +1529,7 @@
       <c r="K31" s="11"/>
     </row>
     <row r="32" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="18"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="5">
         <v>42217</v>
       </c>
@@ -1526,7 +1552,7 @@
       <c r="K32" s="11"/>
     </row>
     <row r="33" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="18"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="5">
         <v>42217</v>
       </c>
@@ -1549,7 +1575,7 @@
       <c r="K33" s="11"/>
     </row>
     <row r="34" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="18"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="5">
         <v>42217</v>
       </c>
@@ -1572,7 +1598,7 @@
       <c r="K34" s="11"/>
     </row>
     <row r="35" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="18"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="5">
         <v>42217</v>
       </c>
@@ -1595,7 +1621,7 @@
       <c r="K35" s="11"/>
     </row>
     <row r="36" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="18"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="5">
         <v>42217</v>
       </c>
@@ -1618,7 +1644,7 @@
       <c r="K36" s="11"/>
     </row>
     <row r="37" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="18"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="5">
         <v>42217</v>
       </c>
@@ -1641,7 +1667,7 @@
       <c r="K37" s="11"/>
     </row>
     <row r="38" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="18"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="5">
         <v>42217</v>
       </c>
@@ -1664,7 +1690,7 @@
       <c r="K38" s="11"/>
     </row>
     <row r="39" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="18"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="5">
         <v>42217</v>
       </c>
@@ -1687,7 +1713,7 @@
       <c r="K39" s="11"/>
     </row>
     <row r="40" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="18"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="5">
         <v>42217</v>
       </c>
@@ -1710,7 +1736,7 @@
       <c r="K40" s="11"/>
     </row>
     <row r="41" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="18"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="5">
         <v>42217</v>
       </c>
@@ -1733,7 +1759,7 @@
       <c r="K41" s="11"/>
     </row>
     <row r="42" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="18"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="5">
         <v>42217</v>
       </c>
@@ -1756,7 +1782,7 @@
       <c r="K42" s="11"/>
     </row>
     <row r="43" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="18"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="5">
         <v>42217</v>
       </c>
@@ -1779,7 +1805,7 @@
       <c r="K43" s="11"/>
     </row>
     <row r="44" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="18"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="5">
         <v>42217</v>
       </c>
@@ -1802,7 +1828,7 @@
       <c r="K44" s="11"/>
     </row>
     <row r="45" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="18"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="5">
         <v>42217</v>
       </c>
@@ -1825,7 +1851,7 @@
       <c r="K45" s="11"/>
     </row>
     <row r="46" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="18"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="5">
         <v>42217</v>
       </c>
@@ -1848,7 +1874,7 @@
       <c r="K46" s="11"/>
     </row>
     <row r="47" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="18"/>
+      <c r="B47" s="12"/>
       <c r="C47" s="5">
         <v>42217</v>
       </c>
@@ -1871,7 +1897,7 @@
       <c r="K47" s="11"/>
     </row>
     <row r="48" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="18"/>
+      <c r="B48" s="12"/>
       <c r="C48" s="5">
         <v>42217</v>
       </c>
@@ -1894,7 +1920,7 @@
       <c r="K48" s="11"/>
     </row>
     <row r="49" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="18"/>
+      <c r="B49" s="12"/>
       <c r="C49" s="5">
         <v>42217</v>
       </c>
@@ -1917,7 +1943,7 @@
       <c r="K49" s="11"/>
     </row>
     <row r="50" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="18"/>
+      <c r="B50" s="12"/>
       <c r="C50" s="5">
         <v>42217</v>
       </c>
@@ -1940,7 +1966,7 @@
       <c r="K50" s="11"/>
     </row>
     <row r="51" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="18"/>
+      <c r="B51" s="12"/>
       <c r="C51" s="5">
         <v>42217</v>
       </c>
@@ -1963,7 +1989,7 @@
       <c r="K51" s="11"/>
     </row>
     <row r="52" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="18"/>
+      <c r="B52" s="12"/>
       <c r="C52" s="5">
         <v>42217</v>
       </c>
@@ -1986,7 +2012,7 @@
       <c r="K52" s="11"/>
     </row>
     <row r="53" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="18"/>
+      <c r="B53" s="12"/>
       <c r="C53" s="5">
         <v>42217</v>
       </c>
@@ -2009,7 +2035,7 @@
       <c r="K53" s="11"/>
     </row>
     <row r="54" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="18"/>
+      <c r="B54" s="12"/>
       <c r="C54" s="5">
         <v>42217</v>
       </c>
@@ -2032,7 +2058,7 @@
       <c r="K54" s="11"/>
     </row>
     <row r="55" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="18"/>
+      <c r="B55" s="12"/>
       <c r="C55" s="5">
         <v>42217</v>
       </c>
@@ -2055,7 +2081,7 @@
       <c r="K55" s="11"/>
     </row>
     <row r="56" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="18"/>
+      <c r="B56" s="12"/>
       <c r="C56" s="5">
         <v>42217</v>
       </c>
@@ -2078,7 +2104,7 @@
       <c r="K56" s="11"/>
     </row>
     <row r="57" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="18"/>
+      <c r="B57" s="12"/>
       <c r="C57" s="5">
         <v>42217</v>
       </c>
@@ -2101,7 +2127,7 @@
       <c r="K57" s="11"/>
     </row>
     <row r="58" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="18"/>
+      <c r="B58" s="12"/>
       <c r="C58" s="5">
         <v>42217</v>
       </c>
@@ -2124,7 +2150,7 @@
       <c r="K58" s="11"/>
     </row>
     <row r="59" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="18"/>
+      <c r="B59" s="12"/>
       <c r="C59" s="5">
         <v>42217</v>
       </c>
@@ -2147,7 +2173,7 @@
       <c r="K59" s="11"/>
     </row>
     <row r="60" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="18"/>
+      <c r="B60" s="12"/>
       <c r="C60" s="5">
         <v>42217</v>
       </c>
@@ -2170,7 +2196,7 @@
       <c r="K60" s="11"/>
     </row>
     <row r="61" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="18"/>
+      <c r="B61" s="12"/>
       <c r="C61" s="5">
         <v>42217</v>
       </c>
@@ -2193,7 +2219,7 @@
       <c r="K61" s="11"/>
     </row>
     <row r="62" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="18"/>
+      <c r="B62" s="12"/>
       <c r="C62" s="5">
         <v>42217</v>
       </c>
@@ -2216,7 +2242,7 @@
       <c r="K62" s="11"/>
     </row>
     <row r="63" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="18"/>
+      <c r="B63" s="12"/>
       <c r="C63" s="5">
         <v>42217</v>
       </c>
@@ -2239,7 +2265,7 @@
       <c r="K63" s="11"/>
     </row>
     <row r="64" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="18"/>
+      <c r="B64" s="12"/>
       <c r="C64" s="5">
         <v>42217</v>
       </c>
@@ -2262,7 +2288,7 @@
       <c r="K64" s="11"/>
     </row>
     <row r="65" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="18"/>
+      <c r="B65" s="12"/>
       <c r="C65" s="5">
         <v>42217</v>
       </c>
@@ -2285,7 +2311,7 @@
       <c r="K65" s="11"/>
     </row>
     <row r="66" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="18"/>
+      <c r="B66" s="12"/>
       <c r="C66" s="5">
         <v>42217</v>
       </c>
@@ -2308,7 +2334,7 @@
       <c r="K66" s="11"/>
     </row>
     <row r="67" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="18"/>
+      <c r="B67" s="12"/>
       <c r="C67" s="5">
         <v>42217</v>
       </c>
@@ -2331,7 +2357,7 @@
       <c r="K67" s="11"/>
     </row>
     <row r="68" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="18"/>
+      <c r="B68" s="12"/>
       <c r="C68" s="5">
         <v>42217</v>
       </c>
@@ -2354,7 +2380,7 @@
       <c r="K68" s="11"/>
     </row>
     <row r="69" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="18"/>
+      <c r="B69" s="12"/>
       <c r="C69" s="5">
         <v>42217</v>
       </c>
@@ -2377,7 +2403,7 @@
       <c r="K69" s="11"/>
     </row>
     <row r="70" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="18"/>
+      <c r="B70" s="12"/>
       <c r="C70" s="5">
         <v>42217</v>
       </c>
@@ -2400,7 +2426,7 @@
       <c r="K70" s="11"/>
     </row>
     <row r="71" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="18"/>
+      <c r="B71" s="12"/>
       <c r="C71" s="5">
         <v>42217</v>
       </c>
@@ -2423,7 +2449,7 @@
       <c r="K71" s="11"/>
     </row>
     <row r="72" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="18"/>
+      <c r="B72" s="12"/>
       <c r="C72" s="5">
         <v>42217</v>
       </c>
@@ -2446,7 +2472,7 @@
       <c r="K72" s="11"/>
     </row>
     <row r="73" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="18"/>
+      <c r="B73" s="12"/>
       <c r="C73" s="5">
         <v>42217</v>
       </c>
@@ -2469,7 +2495,7 @@
       <c r="K73" s="11"/>
     </row>
     <row r="74" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="18"/>
+      <c r="B74" s="12"/>
       <c r="C74" s="5">
         <v>42217</v>
       </c>
@@ -2492,7 +2518,7 @@
       <c r="K74" s="11"/>
     </row>
     <row r="75" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="18"/>
+      <c r="B75" s="12"/>
       <c r="C75" s="5">
         <v>42217</v>
       </c>
@@ -2515,7 +2541,7 @@
       <c r="K75" s="11"/>
     </row>
     <row r="76" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="18"/>
+      <c r="B76" s="12"/>
       <c r="C76" s="5">
         <v>42217</v>
       </c>
@@ -2538,7 +2564,7 @@
       <c r="K76" s="11"/>
     </row>
     <row r="77" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="18"/>
+      <c r="B77" s="12"/>
       <c r="C77" s="5">
         <v>42217</v>
       </c>
@@ -2561,7 +2587,7 @@
       <c r="K77" s="11"/>
     </row>
     <row r="78" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="18"/>
+      <c r="B78" s="12"/>
       <c r="C78" s="5">
         <v>42217</v>
       </c>
@@ -2584,7 +2610,7 @@
       <c r="K78" s="11"/>
     </row>
     <row r="79" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="18"/>
+      <c r="B79" s="12"/>
       <c r="C79" s="5">
         <v>42217</v>
       </c>
@@ -2607,7 +2633,7 @@
       <c r="K79" s="11"/>
     </row>
     <row r="80" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="18"/>
+      <c r="B80" s="12"/>
       <c r="C80" s="5">
         <v>42217</v>
       </c>
@@ -2630,7 +2656,7 @@
       <c r="K80" s="11"/>
     </row>
     <row r="81" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="18"/>
+      <c r="B81" s="12"/>
       <c r="C81" s="5">
         <v>42217</v>
       </c>
@@ -2653,7 +2679,7 @@
       <c r="K81" s="11"/>
     </row>
     <row r="82" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="18"/>
+      <c r="B82" s="12"/>
       <c r="C82" s="5">
         <v>42217</v>
       </c>
@@ -2676,7 +2702,7 @@
       <c r="K82" s="11"/>
     </row>
     <row r="83" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="18"/>
+      <c r="B83" s="12"/>
       <c r="C83" s="5">
         <v>42217</v>
       </c>
@@ -2699,7 +2725,7 @@
       <c r="K83" s="11"/>
     </row>
     <row r="84" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="18"/>
+      <c r="B84" s="12"/>
       <c r="C84" s="5">
         <v>42217</v>
       </c>
@@ -2722,7 +2748,7 @@
       <c r="K84" s="11"/>
     </row>
     <row r="85" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="18"/>
+      <c r="B85" s="12"/>
       <c r="C85" s="5">
         <v>42217</v>
       </c>
@@ -2745,7 +2771,7 @@
       <c r="K85" s="11"/>
     </row>
     <row r="86" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="18"/>
+      <c r="B86" s="12"/>
       <c r="C86" s="5">
         <v>42217</v>
       </c>
@@ -2768,7 +2794,7 @@
       <c r="K86" s="11"/>
     </row>
     <row r="87" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="18"/>
+      <c r="B87" s="12"/>
       <c r="C87" s="5">
         <v>42217</v>
       </c>
@@ -2791,7 +2817,7 @@
       <c r="K87" s="11"/>
     </row>
     <row r="88" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="18"/>
+      <c r="B88" s="12"/>
       <c r="C88" s="5">
         <v>42217</v>
       </c>
@@ -2814,7 +2840,7 @@
       <c r="K88" s="11"/>
     </row>
     <row r="89" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="18"/>
+      <c r="B89" s="12"/>
       <c r="C89" s="5">
         <v>42217</v>
       </c>
@@ -2837,7 +2863,7 @@
       <c r="K89" s="11"/>
     </row>
     <row r="90" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="18"/>
+      <c r="B90" s="12"/>
       <c r="C90" s="5">
         <v>42217</v>
       </c>
@@ -2860,7 +2886,7 @@
       <c r="K90" s="11"/>
     </row>
     <row r="91" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="18"/>
+      <c r="B91" s="12"/>
       <c r="C91" s="5">
         <v>42217</v>
       </c>
@@ -2883,7 +2909,7 @@
       <c r="K91" s="11"/>
     </row>
     <row r="92" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="18"/>
+      <c r="B92" s="12"/>
       <c r="C92" s="5">
         <v>42217</v>
       </c>
@@ -2906,7 +2932,7 @@
       <c r="K92" s="11"/>
     </row>
     <row r="93" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="18"/>
+      <c r="B93" s="12"/>
       <c r="C93" s="5">
         <v>42217</v>
       </c>
@@ -2929,7 +2955,7 @@
       <c r="K93" s="11"/>
     </row>
     <row r="94" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="18"/>
+      <c r="B94" s="12"/>
       <c r="C94" s="5">
         <v>42217</v>
       </c>
@@ -2952,7 +2978,7 @@
       <c r="K94" s="11"/>
     </row>
     <row r="95" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="18"/>
+      <c r="B95" s="12"/>
       <c r="C95" s="5">
         <v>42217</v>
       </c>
@@ -2975,7 +3001,7 @@
       <c r="K95" s="11"/>
     </row>
     <row r="96" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="18"/>
+      <c r="B96" s="12"/>
       <c r="C96" s="5">
         <v>42217</v>
       </c>
@@ -2998,7 +3024,7 @@
       <c r="K96" s="11"/>
     </row>
     <row r="97" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="18"/>
+      <c r="B97" s="12"/>
       <c r="C97" s="5">
         <v>42217</v>
       </c>
@@ -3021,7 +3047,7 @@
       <c r="K97" s="11"/>
     </row>
     <row r="98" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="18"/>
+      <c r="B98" s="12"/>
       <c r="C98" s="5">
         <v>42217</v>
       </c>
@@ -3044,7 +3070,7 @@
       <c r="K98" s="11"/>
     </row>
     <row r="99" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="18"/>
+      <c r="B99" s="12"/>
       <c r="C99" s="5">
         <v>42217</v>
       </c>
@@ -3067,7 +3093,7 @@
       <c r="K99" s="11"/>
     </row>
     <row r="100" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="18"/>
+      <c r="B100" s="12"/>
       <c r="C100" s="5">
         <v>42217</v>
       </c>

</xml_diff>

<commit_message>
Débout d'affichage de la grille et menu aide dans CLion
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
+++ b/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1201,9 @@
       <c r="K17" s="11"/>
     </row>
     <row r="18" spans="2:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
+      <c r="B18" s="12">
+        <v>44246</v>
+      </c>
       <c r="C18" s="5">
         <v>42217.583333333336</v>
       </c>
@@ -1230,20 +1232,24 @@
       <c r="K18" s="11"/>
     </row>
     <row r="19" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
+      <c r="B19" s="12">
+        <v>44258</v>
+      </c>
       <c r="C19" s="5">
-        <v>42217</v>
+        <v>42217.510416666664</v>
       </c>
       <c r="D19" s="5">
-        <v>42217</v>
+        <v>42217.524305555555</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="4"/>
+        <v>1.3888888890505768E-2</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G19" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4" t="s">
@@ -1255,16 +1261,18 @@
     <row r="20" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="C20" s="5">
-        <v>42217</v>
+        <v>42217.524305555555</v>
       </c>
       <c r="D20" s="5">
-        <v>42217</v>
+        <v>42217.590277777781</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="4"/>
+        <v>6.5972222226264421E-2</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G20" s="4" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Petites modifications dans le code et mise à jour du journal de travail.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
+++ b/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1.Modules\MA\20\BatailleNavale\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\CPNV\Modules\MA\MA-20\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85200316-C6E0-45DD-A819-4D81E6EB2D42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Parametres" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -207,12 +217,19 @@
     <t>M.Viret nous a separé par groupe et on a dut fair un exemple de HUD dans un jeu.
 Après 45 minutes, on devait présenter, sauf que on a pas présente un HUD et donc l'exercice était faut.
 Pour une deuxième fois, on devait encore faire un HUD et l'améliorer avec les defauts de la première présentation et ce n'était pas nous que devions le présenter donc il fallait que celá soit bien compréhensible.</t>
+  </si>
+  <si>
+    <t>Amélioration du code de la Bataille Navale</t>
+  </si>
+  <si>
+    <t>Dans cette partie de code, j'ai essayé de corriger les erreurs mais il y toujours quelques problèmes à corriger.
+La grille s'affiche avec des valeures aléatoires et je n'ai pas trouvé le problème.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
@@ -745,11 +762,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1389,27 +1406,35 @@
       </c>
       <c r="K22" s="11"/>
     </row>
-    <row r="23" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
+    <row r="23" spans="2:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="12">
+        <v>44260</v>
+      </c>
       <c r="C23" s="5">
-        <v>42217</v>
+        <v>42217.5625</v>
       </c>
       <c r="D23" s="5">
-        <v>42217</v>
+        <v>42217.625</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="4"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="4"/>
+      <c r="H23" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="I23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="4"/>
+      <c r="J23" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="K23" s="11"/>
     </row>
     <row r="24" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3188,28 +3213,28 @@
     <mergeCell ref="B2:K3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K6" r:id="rId1"/>
-    <hyperlink ref="K15" r:id="rId2"/>
-    <hyperlink ref="K20" r:id="rId3"/>
+    <hyperlink ref="K6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="K20" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Parametres!$D$3:$D$10</xm:f>
           </x14:formula1>
           <xm:sqref>G5:G100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Parametres!$F$3:$F$4</xm:f>
           </x14:formula1>
           <xm:sqref>I5:I100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Parametres!$B$3:$B$5</xm:f>
           </x14:formula1>
@@ -3222,7 +3247,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Sauvegarde du code et du journal de travail
Dans ce code, j'ai commencé a placer les bateaux et j'ai fini le menu d'aide.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
+++ b/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\CPNV\Modules\MA\MA-20\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85200316-C6E0-45DD-A819-4D81E6EB2D42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B578ACEA-1C62-457F-88CC-B0A15E7D1BB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -224,6 +224,17 @@
   <si>
     <t>Dans cette partie de code, j'ai essayé de corriger les erreurs mais il y toujours quelques problèmes à corriger.
 La grille s'affiche avec des valeures aléatoires et je n'ai pas trouvé le problème.</t>
+  </si>
+  <si>
+    <t>Coomencé le débout du menu aide de la bataille navale</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/10882277/properly-print-utf8-characters-in-windows-console</t>
+  </si>
+  <si>
+    <t>Au débout, j'avais recontré des problémes parce que Clion voulait compiler avec le fichier de visual Studio Code et donv je n'avais pas trouvé la solution sur internet mais j'ai réussi a trouver l'erreure.
+Pour afficher les acents sur mon projet, je suis aller chercher le code se trouvant dans sources sur le web.
+J'ai également commencé a faire la map et l'emplacement des bateux, mais pour l'instant ils sont tous sur la même case.</t>
   </si>
 </sst>
 </file>
@@ -765,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -1437,28 +1448,38 @@
       </c>
       <c r="K23" s="11"/>
     </row>
-    <row r="24" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
+    <row r="24" spans="2:11" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="12">
+        <v>44262</v>
+      </c>
       <c r="C24" s="5">
-        <v>42217</v>
+        <v>42217.760416666664</v>
       </c>
       <c r="D24" s="5">
         <v>42217</v>
       </c>
       <c r="E24" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="4"/>
+        <v>-0.76041666666424135</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="4"/>
+      <c r="H24" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="I24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J24" s="4"/>
-      <c r="K24" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="25" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="12"/>
@@ -3216,9 +3237,10 @@
     <hyperlink ref="K6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="K15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="K20" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="K24" r:id="rId4" xr:uid="{2806372D-E53B-4D16-83A4-0BD19672E9E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">

</xml_diff>

<commit_message>
Résolution de problèmes de compilation
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
+++ b/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\CPNV\Modules\MA\MA-20\BatailleNavale\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1.Modules\MA\20\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B578ACEA-1C62-457F-88CC-B0A15E7D1BB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Parametres" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -235,12 +234,21 @@
     <t>Au débout, j'avais recontré des problémes parce que Clion voulait compiler avec le fichier de visual Studio Code et donv je n'avais pas trouvé la solution sur internet mais j'ai réussi a trouver l'erreure.
 Pour afficher les acents sur mon projet, je suis aller chercher le code se trouvant dans sources sur le web.
 J'ai également commencé a faire la map et l'emplacement des bateux, mais pour l'instant ils sont tous sur la même case.</t>
+  </si>
+  <si>
+    <t>https://www.jetbrains.com/help/clion/cmake-cache.html</t>
+  </si>
+  <si>
+    <t>M. Viret, m'a aidé car mon compilateur ne marchait plus, don on à dû reset le Cmakecache.</t>
+  </si>
+  <si>
+    <t>Résolution de problemes de compilation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
@@ -773,11 +781,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1481,28 +1489,38 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
+    <row r="25" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="12">
+        <v>44265</v>
+      </c>
       <c r="C25" s="5">
-        <v>42217</v>
+        <v>42217.5625</v>
       </c>
       <c r="D25" s="5">
-        <v>42217</v>
+        <v>42217.576388888891</v>
       </c>
       <c r="E25" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="4"/>
+        <v>1.3888888890505768E-2</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="I25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="4"/>
-      <c r="K25" s="11"/>
+      <c r="J25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="26" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="12"/>
@@ -3234,29 +3252,30 @@
     <mergeCell ref="B2:K3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="K20" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="K24" r:id="rId4" xr:uid="{2806372D-E53B-4D16-83A4-0BD19672E9E9}"/>
+    <hyperlink ref="K6" r:id="rId1"/>
+    <hyperlink ref="K15" r:id="rId2"/>
+    <hyperlink ref="K20" r:id="rId3"/>
+    <hyperlink ref="K24" r:id="rId4"/>
+    <hyperlink ref="K25" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Parametres!$D$3:$D$10</xm:f>
           </x14:formula1>
           <xm:sqref>G5:G100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Parametres!$F$3:$F$4</xm:f>
           </x14:formula1>
           <xm:sqref>I5:I100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Parametres!$B$3:$B$5</xm:f>
           </x14:formula1>
@@ -3269,7 +3288,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Mise à jour du code
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
+++ b/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1.CPNV\MA-20\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B27F705-CE2C-40BD-8A88-DA207E9AFEB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC069B1-AD6A-4944-959A-DECF54F40F19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="76">
   <si>
     <t>Date</t>
   </si>
@@ -258,6 +258,22 @@
   </si>
   <si>
     <t>Cette partie de cours a été destinée pour nous apprendre le sprint et comment faire un sprint avec quelles informations.</t>
+  </si>
+  <si>
+    <t>MA-20 &amp;
+I-CT 431</t>
+  </si>
+  <si>
+    <t>Questionnaire qualités</t>
+  </si>
+  <si>
+    <t>Revue sur le questionnaire qualités des modules.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Révision du code </t>
+  </si>
+  <si>
+    <t>Dans cette partie du cours j'ai relu le code pour me fixer des objetctifs et ansi commencer les sprints sur GitHub</t>
   </si>
 </sst>
 </file>
@@ -800,7 +816,7 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1796875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1601,7 +1617,7 @@
       </c>
       <c r="K27" s="11"/>
     </row>
-    <row r="28" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:11" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="12">
         <v>44266</v>
       </c>
@@ -1609,44 +1625,58 @@
         <v>42217.395833333336</v>
       </c>
       <c r="D28" s="5">
-        <v>42217</v>
+        <v>42217.447916666664</v>
       </c>
       <c r="E28" s="5">
         <f t="shared" si="6"/>
-        <v>-0.39583333333575865</v>
-      </c>
-      <c r="F28" s="4"/>
+        <v>5.2083333328482695E-2</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G28" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="I28" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J28" s="4"/>
+      <c r="J28" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="K28" s="11"/>
     </row>
-    <row r="29" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="12"/>
+    <row r="29" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="12">
+        <v>44266</v>
+      </c>
       <c r="C29" s="5">
-        <v>42217</v>
+        <v>42217.447916666664</v>
       </c>
       <c r="D29" s="5">
-        <v>42217</v>
+        <v>42217.458333333336</v>
       </c>
       <c r="E29" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="4"/>
+        <v>1.0416666671517305E-2</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="G29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="I29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="K29" s="11"/>
     </row>
     <row r="30" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -3315,7 +3345,7 @@
           <x14:formula1>
             <xm:f>Parametres!$B$3:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F5:F100</xm:sqref>
+          <xm:sqref>F5:F28 F30:F100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Tentative de faire ka deuxième carte
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
+++ b/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\CPNV\Modules\MA\MA-20\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955D49E9-2D03-48CA-8C74-08582E9A7865}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9373EE3A-EFEA-48A3-BC15-20F666479D6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="93">
   <si>
     <t>Date</t>
   </si>
@@ -382,6 +382,123 @@
   <si>
     <t>Début et mise à jour du journal de bord</t>
   </si>
+  <si>
+    <t>Stocker des informations en JSON</t>
+  </si>
+  <si>
+    <t>J'ai fait des recherches de comment je deverais sotcker mes informations sur les scores et temps en JSON mais pas trop de réussites.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Liens que j'ai trouvé pour essayer de comprendre :</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://github.com/netmail-open/wjelement/blob/master/example/validate.c
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>---</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://www.tutorialspoint.com/json/json_quick_guide.htm
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>---</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Liens pour stocker les informations en JSON :</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://realtimelogic.com/downloads/Using-The-JSON-C-API.pdf
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>---</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://stackoverflow.com/questions/33685871/save-an-integer-array-written-in-c-to-a-json-text-file-array</t>
+    </r>
+  </si>
+  <si>
+    <t>J'ai continué de me renseigner pour stocker mes informations dans un fichier JSON.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> j'ai essayé de faire une deuxième carte pour jouer aléatoirement, mais aussi, pas trop de succés.</t>
+  </si>
+  <si>
+    <t>Faire une deuxième carte de jeu</t>
+  </si>
 </sst>
 </file>
 
@@ -391,7 +508,7 @@
     <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +551,12 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -937,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1929,73 +2052,101 @@
       </c>
       <c r="K33" s="11"/>
     </row>
-    <row r="34" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="12"/>
+    <row r="34" spans="2:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="12">
+        <v>44272</v>
+      </c>
       <c r="C34" s="5">
-        <v>42217</v>
+        <v>42217.5625</v>
       </c>
       <c r="D34" s="5">
-        <v>42217</v>
+        <v>42217.625</v>
       </c>
       <c r="E34" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="4"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G34" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="I34" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J34" s="4"/>
-      <c r="K34" s="11"/>
-    </row>
-    <row r="35" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="12"/>
+        <v>23</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="12">
+        <v>44273</v>
+      </c>
       <c r="C35" s="5">
-        <v>42217</v>
+        <v>42217.333333333336</v>
       </c>
       <c r="D35" s="5">
-        <v>42217</v>
+        <v>42217.416666666664</v>
       </c>
       <c r="E35" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="4"/>
+        <v>8.3333333328482695E-2</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="I35" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J35" s="4"/>
-      <c r="K35" s="11"/>
-    </row>
-    <row r="36" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="12"/>
+        <v>23</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="12">
+        <v>44273</v>
+      </c>
       <c r="C36" s="5">
-        <v>42217</v>
+        <v>42217.416666666664</v>
       </c>
       <c r="D36" s="5">
-        <v>42217</v>
+        <v>42217.5</v>
       </c>
       <c r="E36" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="4"/>
+        <v>8.3333333335758653E-2</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G36" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H36" s="4"/>
+      <c r="H36" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="I36" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J36" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="K36" s="11"/>
     </row>
     <row r="37" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Nouvelle carte avec les fichiers avec les grilles au hasard
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
+++ b/Documentation/Journal de travail Bataille Navale Rui_Monteiro.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\CPNV\Modules\MA\MA-20\BatailleNavale\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1.Modules\MA\20\BatailleNavale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9373EE3A-EFEA-48A3-BC15-20F666479D6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Parametres" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -499,11 +498,20 @@
   <si>
     <t>Faire une deuxième carte de jeu</t>
   </si>
+  <si>
+    <t>31.04.2021</t>
+  </si>
+  <si>
+    <t>Refaire le code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai commencé à refaire mon code pour pouvoir afficher une grille plus propre et aussi pour pouvoir prendre un fichier au hasard dans le dossier </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
@@ -1057,11 +1065,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2149,27 +2157,35 @@
       </c>
       <c r="K36" s="11"/>
     </row>
-    <row r="37" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="12"/>
+    <row r="37" spans="2:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="C37" s="5">
-        <v>42217</v>
+        <v>42217.541666666664</v>
       </c>
       <c r="D37" s="5">
-        <v>42217</v>
+        <v>42217.625</v>
       </c>
       <c r="E37" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="4"/>
+        <v>8.3333333335758653E-2</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G37" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H37" s="4"/>
+      <c r="H37" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="I37" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J37" s="4"/>
+      <c r="J37" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="K37" s="11"/>
     </row>
     <row r="38" spans="2:11" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3626,32 +3642,32 @@
     <mergeCell ref="B2:K3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="K15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="K20" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="K24" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="K25" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="K26" r:id="rId6" xr:uid="{E8BAB817-E150-4DE5-AB79-F3DC8E9F7350}"/>
-    <hyperlink ref="K31" r:id="rId7" display="https://cboard.cprogramming.com/cplusplus-programming/117049-setconsoletitle.html" xr:uid="{F50702E1-9B94-4BAD-8264-0497D57E0E42}"/>
+    <hyperlink ref="K6" r:id="rId1"/>
+    <hyperlink ref="K15" r:id="rId2"/>
+    <hyperlink ref="K20" r:id="rId3"/>
+    <hyperlink ref="K24" r:id="rId4"/>
+    <hyperlink ref="K25" r:id="rId5"/>
+    <hyperlink ref="K26" r:id="rId6"/>
+    <hyperlink ref="K31" r:id="rId7" display="https://cboard.cprogramming.com/cplusplus-programming/117049-setconsoletitle.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Parametres!$D$3:$D$10</xm:f>
           </x14:formula1>
           <xm:sqref>G5:G100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Parametres!$F$3:$F$4</xm:f>
           </x14:formula1>
           <xm:sqref>I5:I100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Parametres!$B$3:$B$5</xm:f>
           </x14:formula1>
@@ -3664,7 +3680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>